<commit_message>
pulizia settings codice per simulazione tramite AI ( neat ) e HAND ( a mano)
</commit_message>
<xml_diff>
--- a/Simulation Per Light/SimulationAlgorithm.xlsx
+++ b/Simulation Per Light/SimulationAlgorithm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\SmartTrafficLight\Simulation Per Light\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F178C6F-A6DD-4776-A2AD-317D384F33F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15C4240-D2E5-4E7B-BE93-E6299733D1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2730" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{0D441BBB-1A37-4B96-B7E7-D8E10F23B46D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0D441BBB-1A37-4B96-B7E7-D8E10F23B46D}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,30 +35,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>lane</t>
   </si>
@@ -81,19 +59,13 @@
     <t>out</t>
   </si>
   <si>
-    <t>coppie</t>
-  </si>
-  <si>
-    <t>coppie ordinate</t>
-  </si>
-  <si>
     <t>bonus</t>
   </si>
   <si>
     <t>outIndex</t>
   </si>
   <si>
-    <t>possibili</t>
+    <t>time green</t>
   </si>
 </sst>
 </file>
@@ -445,29 +417,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795FC95A-3380-4623-A4F5-3111AAD2BB20}">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K2">
-        <f>MATCH(K4,A4:N4)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>MATCH(O4,A4:R4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -484,114 +456,92 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" t="s">
         <v>9</v>
       </c>
       <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
         <v>6</v>
       </c>
-      <c r="O4" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>6</v>
-      </c>
-      <c r="T4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f>(C5 - $D$12) / ($D$13 - $D$12)</f>
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
         <v>40</v>
       </c>
       <c r="G5">
         <f>(F5 - $G$12) / ($G$13 - $G$12)</f>
-        <v>0.66666666666666663</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H5">
-        <f>IF(F5&gt;G13,G5*2,G5)</f>
-        <v>0.66666666666666663</v>
+        <f>IF(F5&gt;$G$13,G5+(F5-$G$13),G5)</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="K5">
-        <f>H5*D5</f>
-        <v>0.6</v>
+        <f>(J5 - $K$12) / ($K$13 - $K$12)</f>
+        <v>5.5552469307260709E-5</v>
       </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
-      <c r="Q5">
-        <f>VLOOKUP(O5,$A$5:$K$10,$K$2)+VLOOKUP(P5,$A$5:$K$10,$K$2)</f>
-        <v>1.7666666666666666</v>
-      </c>
-      <c r="T5" cm="1">
-        <f t="array" ref="T5:U10">_xlfn.CHOOSECOLS( _xlfn._xlws.SORT(O5:Q10,3,-1),1,2)</f>
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <f>H5*D5+D5*K5</f>
+        <v>5.5583331790209183E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" ref="D6:D10" si="0">(C6 - $D$12) / ($D$13 - $D$12)</f>
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
         <v>50</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G10" si="1">(F6 - $G$12) / ($G$13 - $G$12)</f>
-        <v>0.83333333333333337</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H10" si="2">IF(F6&gt;G14,G6*2,G6)</f>
-        <v>1.6666666666666667</v>
+        <f t="shared" ref="H6:H10" si="2">IF(F6&gt;$G$13,G6+(F6-$G$13),G6)</f>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K10" si="3">H6*D6</f>
-        <v>1.1666666666666667</v>
+        <f t="shared" ref="K6:K10" si="3">(J6 - $K$12) / ($K$13 - $K$12)</f>
+        <v>5.5552469307260709E-5</v>
       </c>
       <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6">
-        <v>4</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" ref="Q6:Q9" si="4">VLOOKUP(O6,$A$5:$K$10,$K$2)+VLOOKUP(P6,$A$5:$K$10,$K$2)</f>
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>2</v>
-      </c>
-      <c r="U6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="O6:O10" si="4">H6*D6+D6*K6</f>
+        <v>6.9472220679098085E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -608,33 +558,24 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J7">
+        <v>-1</v>
+      </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-5.4996944614188106E-3</v>
       </c>
       <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>3</v>
-      </c>
-      <c r="Q7">
         <f t="shared" si="4"/>
-        <v>0.6</v>
-      </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-      <c r="U7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>-5.4996944614188106E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -651,28 +592,19 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.2276540192211543E-2</v>
       </c>
       <c r="O8">
-        <v>2</v>
-      </c>
-      <c r="P8">
-        <v>4</v>
-      </c>
-      <c r="Q8">
         <f t="shared" si="4"/>
-        <v>1.1666666666666667</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2.2276540192211543E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -681,41 +613,32 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>5.5552469307260709E-5</v>
       </c>
       <c r="O9">
-        <v>5</v>
-      </c>
-      <c r="P9">
-        <v>6</v>
-      </c>
-      <c r="Q9">
         <f t="shared" si="4"/>
-        <v>0.8</v>
-      </c>
-      <c r="T9">
-        <v>3</v>
-      </c>
-      <c r="U9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>7.7805554012431416E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -724,31 +647,32 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>120</v>
+        <v>362</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.0055555555555555</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>IF(F10&gt;$G$13,G10+(F10-$G$13),G10)</f>
+        <v>3.0055555555555555</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
-        <v>0.4</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>5.5552469307260709E-5</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="4"/>
+        <v>1.5028055540124314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>3</v>
       </c>
@@ -761,36 +685,32 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13">
         <f>MAX(C5:C10)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
       </c>
       <c r="G13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
+        <v>360</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>